<commit_message>
Updated Mass List and Parameters file
</commit_message>
<xml_diff>
--- a/Mass List and Parameters.xlsx
+++ b/Mass List and Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Erick\MSI-CE-MS-Data-Preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F5F980-0B44-4645-ADC7-11ED9D3A998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B38767-500B-4F22-9463-BC4701FC03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3F442743-5A66-4E15-9366-B88AC1790E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{3F442743-5A66-4E15-9366-B88AC1790E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyte Mass List" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -289,9 +289,6 @@
     <t>required.points.for.peak.picking</t>
   </si>
   <si>
-    <t>eie.smoothing.strength</t>
-  </si>
-  <si>
     <t>ref.mass.one</t>
   </si>
   <si>
@@ -311,6 +308,24 @@
   </si>
   <si>
     <t>peak.fwhm.tolerance.multiplier</t>
+  </si>
+  <si>
+    <t>smoothing.kernal</t>
+  </si>
+  <si>
+    <t>smoothing.strength</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Creatine, Isoleucine, Leucine</t>
+  </si>
+  <si>
+    <t>Internal Standard</t>
+  </si>
+  <si>
+    <t>class</t>
   </si>
 </sst>
 </file>
@@ -726,29 +741,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A9B2B3-45F3-4E9C-8863-F19858D470D6}">
-  <dimension ref="A1:Y48"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="23" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="25" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -780,46 +797,52 @@
         <v>74</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -844,48 +867,54 @@
       <c r="J2" s="1">
         <v>3</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="1">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2">
         <v>0.8556342795252494</v>
       </c>
-      <c r="L2" s="2">
+      <c r="N2" s="2">
         <v>0.86338725941514316</v>
       </c>
-      <c r="M2" s="2">
+      <c r="O2" s="2">
         <v>0.87006564924546004</v>
       </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>0.87630662020905925</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>0.88157363276516687</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <v>0.88838969023409797</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="S2" s="2">
         <v>0.89292447385633489</v>
       </c>
-      <c r="R2" s="2">
+      <c r="T2" s="2">
         <v>0.89738581730769229</v>
       </c>
-      <c r="S2" s="2">
+      <c r="U2" s="2">
         <v>0.90275330396475784</v>
       </c>
-      <c r="T2" s="2">
+      <c r="V2" s="2">
         <v>0.90673463526708775</v>
       </c>
-      <c r="U2" s="2">
+      <c r="W2" s="2">
         <v>0.91102052291256674</v>
       </c>
-      <c r="V2" s="2">
+      <c r="X2" s="2">
         <v>0.91512940528634357</v>
       </c>
-      <c r="W2" s="2">
+      <c r="Y2" s="2">
         <v>0.91914936640603928</v>
       </c>
-      <c r="Y2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -910,48 +939,54 @@
       <c r="J3" s="1">
         <v>3</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2">
         <v>0.96623563218390807</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>0.96797219291167524</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>0.97046288623179833</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>0.9726213372553455</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>0.9738593927585647</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <v>0.97492211838006226</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="S3" s="2">
         <v>0.97588135423948863</v>
       </c>
-      <c r="R3" s="2">
+      <c r="T3" s="2">
         <v>0.97677102871158561</v>
       </c>
-      <c r="S3" s="2">
+      <c r="U3" s="2">
         <v>0.9775963634676933</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>0.97906674436326135</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <v>0.97979009454419286</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>0.97971270161290325</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <v>0.98033227461519667</v>
       </c>
-      <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -982,47 +1017,53 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
         <v>0.99639895242252297</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>0.99662731871838117</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="2">
         <v>0.99845412385195964</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>0.9971421366731108</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <v>0.99733959311424114</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R4" s="2">
         <v>0.99751152748298322</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="S4" s="2">
         <v>0.99656262890141623</v>
       </c>
-      <c r="R4" s="2">
+      <c r="T4" s="2">
         <v>0.99779392681027768</v>
       </c>
-      <c r="S4" s="2">
+      <c r="U4" s="2">
         <v>0.99895564565671457</v>
       </c>
-      <c r="T4" s="2">
+      <c r="V4" s="2">
         <v>1.0019832011199254</v>
       </c>
-      <c r="U4" s="2">
+      <c r="W4" s="2">
         <v>0.99629034937157412</v>
       </c>
-      <c r="V4" s="2">
+      <c r="X4" s="2">
         <v>0.99825949367088596</v>
       </c>
-      <c r="W4" s="2">
+      <c r="Y4" s="2">
         <v>0.99833836858006053</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -1047,47 +1088,53 @@
       <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2">
         <v>1.0064753068522276</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>1.005957144127323</v>
       </c>
-      <c r="M5" s="2">
+      <c r="O5" s="2">
         <v>1.0054334403556433</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>1.0038375930616319</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>1.0047495682210708</v>
       </c>
-      <c r="P5" s="2">
+      <c r="R5" s="2">
         <v>1.0045386803956105</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="S5" s="2">
         <v>1.0053164232641558</v>
       </c>
-      <c r="R5" s="2">
+      <c r="T5" s="2">
         <v>1.0030343488287412</v>
       </c>
-      <c r="S5" s="2">
+      <c r="U5" s="2">
         <v>1.0028855032317636</v>
       </c>
-      <c r="T5" s="2">
+      <c r="V5" s="2">
         <v>1.0036859767838477</v>
       </c>
-      <c r="U5" s="2">
+      <c r="W5" s="2">
         <v>1.0035213118200452</v>
       </c>
-      <c r="V5" s="2">
+      <c r="X5" s="2">
         <v>1.00337361530715</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <v>1.0032378098874015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1112,47 +1159,53 @@
       <c r="J6" s="1">
         <v>3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="1">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
         <v>1.0837904911180773</v>
       </c>
-      <c r="L6" s="2">
+      <c r="N6" s="2">
         <v>1.0786419216684253</v>
       </c>
-      <c r="M6" s="2">
+      <c r="O6" s="2">
         <v>1.0739907659524091</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>1.0696911415318475</v>
       </c>
-      <c r="O6" s="2">
+      <c r="Q6" s="2">
         <v>1.0640255452725009</v>
       </c>
-      <c r="P6" s="2">
+      <c r="R6" s="2">
         <v>1.0597092419522325</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="S6" s="2">
         <v>1.0557774892639569</v>
       </c>
-      <c r="R6" s="2">
+      <c r="T6" s="2">
         <v>1.0520848362429664</v>
       </c>
-      <c r="S6" s="2">
+      <c r="U6" s="2">
         <v>1.0487035576789276</v>
       </c>
-      <c r="T6" s="2">
+      <c r="V6" s="2">
         <v>1.0455421578735038</v>
       </c>
-      <c r="U6" s="2">
+      <c r="W6" s="2">
         <v>1.0426316245988378</v>
       </c>
-      <c r="V6" s="2">
+      <c r="X6" s="2">
         <v>1.039188508064516</v>
       </c>
-      <c r="W6" s="2">
+      <c r="Y6" s="2">
         <v>1.0366072155713006</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
@@ -1177,47 +1230,53 @@
       <c r="J7" s="1">
         <v>3</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
         <v>1.181687565308255</v>
       </c>
-      <c r="L7" s="2">
+      <c r="N7" s="2">
         <v>1.1685804729687792</v>
       </c>
-      <c r="M7" s="2">
+      <c r="O7" s="2">
         <v>1.1568012312063456</v>
       </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2">
         <v>1.1469623260549835</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>1.137035232992369</v>
       </c>
-      <c r="P7" s="2">
+      <c r="R7" s="2">
         <v>1.1280373831775699</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="S7" s="2">
         <v>1.119794267452312</v>
       </c>
-      <c r="R7" s="2">
+      <c r="T7" s="2">
         <v>1.1121531284566921</v>
       </c>
-      <c r="S7" s="2">
+      <c r="U7" s="2">
         <v>1.1058954496961824</v>
       </c>
-      <c r="T7" s="2">
+      <c r="V7" s="2">
         <v>1.1000493074543907</v>
       </c>
-      <c r="U7" s="2">
+      <c r="W7" s="2">
         <v>1.0939370283632579</v>
       </c>
-      <c r="V7" s="2">
+      <c r="X7" s="2">
         <v>1.0867775537634408</v>
       </c>
-      <c r="W7" s="2">
+      <c r="Y7" s="2">
         <v>1.0827428943725059</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1242,47 +1301,53 @@
       <c r="J8" s="1">
         <v>3</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="1">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
         <v>0.99503179650238471</v>
       </c>
-      <c r="L8" s="2">
+      <c r="N8" s="2">
         <v>0.9969807868252516</v>
       </c>
-      <c r="M8" s="2">
+      <c r="O8" s="2">
         <v>0.99721048182586647</v>
       </c>
-      <c r="N8" s="2">
+      <c r="P8" s="2">
         <v>0.99740423188861804</v>
       </c>
-      <c r="O8" s="2">
+      <c r="Q8" s="2">
         <v>0.99632244777875845</v>
       </c>
-      <c r="P8" s="2">
+      <c r="R8" s="2">
         <v>0.99654266353201504</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="S8" s="2">
         <v>0.99784707724425892</v>
       </c>
-      <c r="R8" s="2">
+      <c r="T8" s="2">
         <v>0.99796019285449367</v>
       </c>
-      <c r="S8" s="2">
+      <c r="U8" s="2">
         <v>0.99806383478056782</v>
       </c>
-      <c r="T8" s="2">
+      <c r="V8" s="2">
         <v>0.99815920120488644</v>
       </c>
-      <c r="U8" s="2">
+      <c r="W8" s="2">
         <v>0.99824561403508782</v>
       </c>
-      <c r="V8" s="2">
+      <c r="X8" s="2">
         <v>0.99746102676077786</v>
       </c>
-      <c r="W8" s="2">
+      <c r="Y8" s="2">
         <v>0.99834630350194553</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1307,47 +1372,53 @@
       <c r="J9" s="1">
         <v>3</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="1">
+        <v>4</v>
+      </c>
+      <c r="M9" s="2">
         <v>0.87066203348526561</v>
       </c>
-      <c r="L9" s="2">
+      <c r="N9" s="2">
         <v>0.87728528212547685</v>
       </c>
-      <c r="M9" s="2">
+      <c r="O9" s="2">
         <v>0.88353653337880467</v>
       </c>
-      <c r="N9" s="2">
+      <c r="P9" s="2">
         <v>0.88875062220009948</v>
       </c>
-      <c r="O9" s="2">
+      <c r="Q9" s="2">
         <v>0.8936909281848292</v>
       </c>
-      <c r="P9" s="2">
+      <c r="R9" s="2">
         <v>0.89891227240482396</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="S9" s="2">
         <v>0.90385133315378408</v>
       </c>
-      <c r="R9" s="2">
+      <c r="T9" s="2">
         <v>0.90737680288461542</v>
       </c>
-      <c r="S9" s="2">
+      <c r="U9" s="2">
         <v>0.91193098384728355</v>
       </c>
-      <c r="T9" s="2">
+      <c r="V9" s="2">
         <v>0.91509908098793791</v>
       </c>
-      <c r="U9" s="2">
+      <c r="W9" s="2">
         <v>0.91920860275513072</v>
       </c>
-      <c r="V9" s="2">
+      <c r="X9" s="2">
         <v>0.92259774229074887</v>
       </c>
-      <c r="W9" s="2">
+      <c r="Y9" s="2">
         <v>0.92588972768940414</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1372,11 +1443,11 @@
       <c r="J10" s="1">
         <v>3</v>
       </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1</v>
+      <c r="K10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4</v>
       </c>
       <c r="M10" s="2">
         <v>1</v>
@@ -1388,14 +1459,14 @@
         <v>1</v>
       </c>
       <c r="P10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2">
         <v>0.99899547965846314</v>
       </c>
-      <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2">
-        <v>1</v>
-      </c>
       <c r="S10" s="2">
         <v>1</v>
       </c>
@@ -1411,8 +1482,14 @@
       <c r="W10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1437,47 +1514,53 @@
       <c r="J11" s="1">
         <v>3</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="1">
+        <v>4</v>
+      </c>
+      <c r="M11" s="2">
         <v>0.95338237285076055</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>0.95615765706519351</v>
       </c>
-      <c r="M11" s="2">
+      <c r="O11" s="2">
         <v>0.95809531929405756</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>0.95993031358885017</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <v>0.96162856450440259</v>
       </c>
-      <c r="P11" s="2">
+      <c r="R11" s="2">
         <v>0.9639000551745881</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="S11" s="2">
         <v>0.96537262898695708</v>
       </c>
-      <c r="R11" s="2">
+      <c r="T11" s="2">
         <v>0.96619591346153855</v>
       </c>
-      <c r="S11" s="2">
+      <c r="U11" s="2">
         <v>0.96820851688693099</v>
       </c>
-      <c r="T11" s="2">
+      <c r="V11" s="2">
         <v>0.96952182653647334</v>
       </c>
-      <c r="U11" s="2">
+      <c r="W11" s="2">
         <v>0.97072673601349457</v>
       </c>
-      <c r="V11" s="2">
+      <c r="X11" s="2">
         <v>0.97191629955947123</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y11" s="2">
         <v>0.97361148557562682</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1508,47 +1591,53 @@
       <c r="J12" s="1">
         <v>3</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="1">
+        <v>4</v>
+      </c>
+      <c r="M12" s="2">
         <v>0.85640146215984481</v>
       </c>
-      <c r="L12" s="2">
+      <c r="N12" s="2">
         <v>0.86338725941514316</v>
       </c>
-      <c r="M12" s="2">
+      <c r="O12" s="2">
         <v>0.87006564924546004</v>
       </c>
-      <c r="N12" s="2">
+      <c r="P12" s="2">
         <v>0.87630662020905925</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <v>0.88157363276516687</v>
       </c>
-      <c r="P12" s="2">
+      <c r="R12" s="2">
         <v>0.88771971309214159</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="S12" s="2">
         <v>0.89292447385633489</v>
       </c>
-      <c r="R12" s="2">
+      <c r="T12" s="2">
         <v>0.89738581730769229</v>
       </c>
-      <c r="S12" s="2">
+      <c r="U12" s="2">
         <v>0.90275330396475784</v>
       </c>
-      <c r="T12" s="2">
+      <c r="V12" s="2">
         <v>0.90673463526708775</v>
       </c>
-      <c r="U12" s="2">
+      <c r="W12" s="2">
         <v>0.91102052291256674</v>
       </c>
-      <c r="V12" s="2">
+      <c r="X12" s="2">
         <v>0.91512940528634357</v>
       </c>
-      <c r="W12" s="2">
+      <c r="Y12" s="2">
         <v>0.91914936640603928</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1579,47 +1668,53 @@
       <c r="J13" s="1">
         <v>3</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13" s="2">
         <v>1.0165169908389367</v>
       </c>
-      <c r="L13" s="2">
+      <c r="N13" s="2">
         <v>1.0174930948309877</v>
       </c>
-      <c r="M13" s="2">
+      <c r="O13" s="2">
         <v>1.0135135135135136</v>
       </c>
-      <c r="N13" s="2">
+      <c r="P13" s="2">
         <v>1.0165920026547204</v>
       </c>
-      <c r="O13" s="2">
+      <c r="Q13" s="2">
         <v>1.0114306486792148</v>
       </c>
-      <c r="P13" s="2">
+      <c r="R13" s="2">
         <v>1.0111531488925674</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="S13" s="2">
         <v>1.0108883844407681</v>
       </c>
-      <c r="R13" s="2">
+      <c r="T13" s="2">
         <v>1.0093900240384615</v>
       </c>
-      <c r="S13" s="2">
+      <c r="U13" s="2">
         <v>1.0098017621145376</v>
       </c>
-      <c r="T13" s="2">
+      <c r="V13" s="2">
         <v>1.0089747271682941</v>
       </c>
-      <c r="U13" s="2">
+      <c r="W13" s="2">
         <v>1.0087854933933089</v>
       </c>
-      <c r="V13" s="2">
+      <c r="X13" s="2">
         <v>1.0086040748898679</v>
       </c>
-      <c r="W13" s="2">
+      <c r="Y13" s="2">
         <v>1.0084254516042059</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1644,47 +1739,53 @@
       <c r="J14" s="1">
         <v>3</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="1">
+        <v>4</v>
+      </c>
+      <c r="M14" s="2">
         <v>0.92630533868856901</v>
       </c>
-      <c r="L14" s="2">
+      <c r="N14" s="2">
         <v>0.93059757113420127</v>
       </c>
-      <c r="M14" s="2">
+      <c r="O14" s="2">
         <v>0.93324239065563985</v>
       </c>
-      <c r="N14" s="2">
+      <c r="P14" s="2">
         <v>0.93641114982578388</v>
       </c>
-      <c r="O14" s="2">
+      <c r="Q14" s="2">
         <v>0.93876726714597314</v>
       </c>
-      <c r="P14" s="2">
+      <c r="R14" s="2">
         <v>0.94222432411129509</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="S14" s="2">
         <v>0.94551960293947901</v>
       </c>
-      <c r="R14" s="2">
+      <c r="T14" s="2">
         <v>0.94681490384615385</v>
       </c>
-      <c r="S14" s="2">
+      <c r="U14" s="2">
         <v>0.94922907488986785</v>
       </c>
-      <c r="T14" s="2">
+      <c r="V14" s="2">
         <v>0.95096209075244098</v>
       </c>
-      <c r="U14" s="2">
+      <c r="W14" s="2">
         <v>0.95375316277762168</v>
       </c>
-      <c r="V14" s="2">
+      <c r="X14" s="2">
         <v>0.95584388766519823</v>
       </c>
-      <c r="W14" s="2">
+      <c r="Y14" s="2">
         <v>0.95790644378538681</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1709,47 +1810,53 @@
       <c r="J15" s="1">
         <v>2</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="1">
+        <v>4</v>
+      </c>
+      <c r="M15" s="2">
         <v>1.0326541274817136</v>
       </c>
-      <c r="L15" s="2">
+      <c r="N15" s="2">
         <v>1.0310346967910125</v>
       </c>
-      <c r="M15" s="2">
+      <c r="O15" s="2">
         <v>1.0306025807979167</v>
       </c>
-      <c r="N15" s="2">
+      <c r="P15" s="2">
         <v>1.0273220952596447</v>
       </c>
-      <c r="O15" s="2">
+      <c r="Q15" s="2">
         <v>1.0261406072414354</v>
       </c>
-      <c r="P15" s="2">
+      <c r="R15" s="2">
         <v>1.0242471443406023</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="S15" s="2">
         <v>1.0224707879756316</v>
       </c>
-      <c r="R15" s="2">
+      <c r="T15" s="2">
         <v>1.020824315875535</v>
       </c>
-      <c r="S15" s="2">
+      <c r="U15" s="2">
         <v>1.0193422700496311</v>
       </c>
-      <c r="T15" s="2">
+      <c r="V15" s="2">
         <v>1.0179299834147653</v>
       </c>
-      <c r="U15" s="2">
+      <c r="W15" s="2">
         <v>1.0173475583311649</v>
       </c>
-      <c r="V15" s="2">
+      <c r="X15" s="2">
         <v>1.0154149865591398</v>
       </c>
-      <c r="W15" s="2">
+      <c r="Y15" s="2">
         <v>1.0142519749165242</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1763,7 +1870,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="F16" s="1">
         <v>6</v>
@@ -1780,47 +1887,53 @@
       <c r="J16" s="1">
         <v>3</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+      <c r="M16" s="2">
         <v>1.0246772486772486</v>
       </c>
-      <c r="L16" s="2">
+      <c r="N16" s="2">
         <v>1.0247341083353945</v>
       </c>
-      <c r="M16" s="2">
+      <c r="O16" s="2">
         <v>1.0227948862265819</v>
       </c>
-      <c r="N16" s="2">
+      <c r="P16" s="2">
         <v>1.0222579885373322</v>
       </c>
-      <c r="O16" s="2">
+      <c r="Q16" s="2">
         <v>1.0217074480325228</v>
       </c>
-      <c r="P16" s="2">
+      <c r="R16" s="2">
         <v>1.0212191647296993</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="S16" s="2">
         <v>1.0195431379019544</v>
       </c>
-      <c r="R16" s="2">
+      <c r="T16" s="2">
         <v>1.0179385067986941</v>
       </c>
-      <c r="S16" s="2">
+      <c r="U16" s="2">
         <v>1.0175604959084044</v>
       </c>
-      <c r="T16" s="2">
+      <c r="V16" s="2">
         <v>1.0172182237680361</v>
       </c>
-      <c r="U16" s="2">
+      <c r="W16" s="2">
         <v>1.0163054486530281</v>
       </c>
-      <c r="V16" s="2">
+      <c r="X16" s="2">
         <v>1.0160238371130608</v>
       </c>
-      <c r="W16" s="2">
+      <c r="Y16" s="2">
         <v>1.0151352755854364</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
@@ -1845,47 +1958,53 @@
       <c r="J17" s="1">
         <v>3</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4</v>
+      </c>
+      <c r="M17" s="2">
         <v>1.054401776384535</v>
       </c>
-      <c r="L17" s="2">
+      <c r="N17" s="2">
         <v>1.0507106945565141</v>
       </c>
-      <c r="M17" s="2">
+      <c r="O17" s="2">
         <v>1.0483603646264947</v>
       </c>
-      <c r="N17" s="2">
+      <c r="P17" s="2">
         <v>1.0451974205226835</v>
       </c>
-      <c r="O17" s="2">
+      <c r="Q17" s="2">
         <v>1.0423770092547493</v>
       </c>
-      <c r="P17" s="2">
+      <c r="R17" s="2">
         <v>1.0389408099688473</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="S17" s="2">
         <v>1.0374513132927194</v>
       </c>
-      <c r="R17" s="2">
+      <c r="T17" s="2">
         <v>1.0336170826720532</v>
       </c>
-      <c r="S17" s="2">
+      <c r="U17" s="2">
         <v>1.0316805046616262</v>
       </c>
-      <c r="T17" s="2">
+      <c r="V17" s="2">
         <v>1.0298534223855844</v>
       </c>
-      <c r="U17" s="2">
+      <c r="W17" s="2">
         <v>1.028189782288143</v>
       </c>
-      <c r="V17" s="2">
+      <c r="X17" s="2">
         <v>1.0265877016129032</v>
       </c>
-      <c r="W17" s="2">
+      <c r="Y17" s="2">
         <v>1.0244319569997558</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1910,47 +2029,53 @@
       <c r="J18" s="1">
         <v>3</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="1">
+        <v>4</v>
+      </c>
+      <c r="M18" s="2">
         <v>0.87142921611986102</v>
       </c>
-      <c r="L18" s="2">
+      <c r="N18" s="2">
         <v>0.87873207944232534</v>
       </c>
-      <c r="M18" s="2">
+      <c r="O18" s="2">
         <v>0.8856680023872453</v>
       </c>
-      <c r="N18" s="2">
+      <c r="P18" s="2">
         <v>0.89148830263812839</v>
       </c>
-      <c r="O18" s="2">
+      <c r="Q18" s="2">
         <v>0.89704337991760241</v>
       </c>
-      <c r="P18" s="2">
+      <c r="R18" s="2">
         <v>0.90151336013241901</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="S18" s="2">
         <v>0.90639067369474047</v>
       </c>
-      <c r="R18" s="2">
+      <c r="T18" s="2">
         <v>0.90989332932692313</v>
       </c>
-      <c r="S18" s="2">
+      <c r="U18" s="2">
         <v>0.91439060205580036</v>
       </c>
-      <c r="T18" s="2">
+      <c r="V18" s="2">
         <v>0.91746840896036752</v>
       </c>
-      <c r="U18" s="2">
+      <c r="W18" s="2">
         <v>0.92212538656170928</v>
       </c>
-      <c r="V18" s="2">
+      <c r="X18" s="2">
         <v>0.92545429515418498</v>
       </c>
-      <c r="W18" s="2">
+      <c r="Y18" s="2">
         <v>0.9287206794284173</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1975,47 +2100,53 @@
       <c r="J19" s="1">
         <v>3</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="1">
+        <v>4</v>
+      </c>
+      <c r="M19" s="2">
         <v>0.88645697007987734</v>
       </c>
-      <c r="L19" s="2">
+      <c r="N19" s="2">
         <v>0.89263010215265892</v>
       </c>
-      <c r="M19" s="2">
+      <c r="O19" s="2">
         <v>0.89845681643788911</v>
       </c>
-      <c r="N19" s="2">
+      <c r="P19" s="2">
         <v>0.90256346441015434</v>
       </c>
-      <c r="O19" s="2">
+      <c r="Q19" s="2">
         <v>0.90714112610065434</v>
       </c>
-      <c r="P19" s="2">
+      <c r="R19" s="2">
         <v>0.912035942303145</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="S19" s="2">
         <v>0.91600938786503017</v>
       </c>
-      <c r="R19" s="2">
+      <c r="T19" s="2">
         <v>0.91928335336538469</v>
       </c>
-      <c r="S19" s="2">
+      <c r="U19" s="2">
         <v>0.92356828193832607</v>
       </c>
-      <c r="T19" s="2">
+      <c r="V19" s="2">
         <v>0.92705341757610571</v>
       </c>
-      <c r="U19" s="2">
+      <c r="W19" s="2">
         <v>0.9303486083778465</v>
       </c>
-      <c r="V19" s="2">
+      <c r="X19" s="2">
         <v>0.93347329295154191</v>
       </c>
-      <c r="W19" s="2">
+      <c r="Y19" s="2">
         <v>0.93711242922620652</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2046,47 +2177,53 @@
       <c r="J20" s="1">
         <v>3</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="1">
+        <v>4</v>
+      </c>
+      <c r="M20" s="2">
         <v>0.9232440602711256</v>
       </c>
-      <c r="L20" s="2">
+      <c r="N20" s="2">
         <v>0.92660215446412264</v>
       </c>
-      <c r="M20" s="2">
+      <c r="O20" s="2">
         <v>0.93114725119321196</v>
       </c>
-      <c r="N20" s="2">
+      <c r="P20" s="2">
         <v>0.93536773529915995</v>
       </c>
-      <c r="O20" s="2">
+      <c r="Q20" s="2">
         <v>0.93800931315483116</v>
       </c>
-      <c r="P20" s="2">
+      <c r="R20" s="2">
         <v>0.94114320339325386</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="S20" s="2">
         <v>0.94339919085588597</v>
       </c>
-      <c r="R20" s="2">
+      <c r="T20" s="2">
         <v>0.94560813393471455</v>
       </c>
-      <c r="S20" s="2">
+      <c r="U20" s="2">
         <v>0.94879439496142814</v>
       </c>
-      <c r="T20" s="2">
+      <c r="V20" s="2">
         <v>0.95004181362033235</v>
       </c>
-      <c r="U20" s="2">
+      <c r="W20" s="2">
         <v>0.9530667991060342</v>
       </c>
-      <c r="V20" s="2">
+      <c r="X20" s="2">
         <v>0.95527511007870192</v>
       </c>
-      <c r="W20" s="2">
+      <c r="Y20" s="2">
         <v>0.9574085996001761</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -2112,21 +2249,21 @@
       <c r="J21" s="1">
         <v>3</v>
       </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1</v>
+      <c r="K21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="1">
+        <v>4</v>
       </c>
       <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
         <v>1.0013171976619741</v>
       </c>
-      <c r="N21" s="2">
-        <v>1</v>
-      </c>
-      <c r="O21" s="2">
-        <v>1</v>
-      </c>
       <c r="P21" s="2">
         <v>1</v>
       </c>
@@ -2137,22 +2274,28 @@
         <v>1</v>
       </c>
       <c r="S21" s="2">
+        <v>1</v>
+      </c>
+      <c r="T21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
         <v>0.99901892890120036</v>
       </c>
-      <c r="T21" s="2">
-        <v>1</v>
-      </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
       <c r="V21" s="2">
         <v>1</v>
       </c>
       <c r="W21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -2183,47 +2326,53 @@
       <c r="J22" s="1">
         <v>3</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="1">
+        <v>4</v>
+      </c>
+      <c r="M22" s="2">
         <v>0.98424111948331539</v>
       </c>
-      <c r="L22" s="2">
+      <c r="N22" s="2">
         <v>0.98599110812851276</v>
       </c>
-      <c r="M22" s="2">
+      <c r="O22" s="2">
         <v>0.98569969356486209</v>
       </c>
-      <c r="N22" s="2">
+      <c r="P22" s="2">
         <v>0.98606021985024683</v>
       </c>
-      <c r="O22" s="2">
+      <c r="Q22" s="2">
         <v>0.9877157518270876</v>
       </c>
-      <c r="P22" s="2">
+      <c r="R22" s="2">
         <v>0.98795775717975987</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="S22" s="2">
         <v>0.98822611796166993</v>
       </c>
-      <c r="R22" s="2">
+      <c r="T22" s="2">
         <v>0.98967535536408902</v>
       </c>
-      <c r="S22" s="2">
+      <c r="U22" s="2">
         <v>0.990505991537176</v>
       </c>
-      <c r="T22" s="2">
+      <c r="V22" s="2">
         <v>0.99073364453424373</v>
       </c>
-      <c r="U22" s="2">
+      <c r="W22" s="2">
         <v>0.99034327441479553</v>
       </c>
-      <c r="V22" s="2">
+      <c r="X22" s="2">
         <v>0.99106694770651416</v>
       </c>
-      <c r="W22" s="2">
+      <c r="Y22" s="2">
         <v>0.99124274328446327</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -2248,47 +2397,53 @@
       <c r="J23" s="1">
         <v>3</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="1">
+        <v>4</v>
+      </c>
+      <c r="M23" s="2">
         <v>1.1036613756613758</v>
       </c>
-      <c r="L23" s="2">
+      <c r="N23" s="2">
         <v>1.0968340341330696</v>
       </c>
-      <c r="M23" s="2">
+      <c r="O23" s="2">
         <v>1.0917825842244915</v>
       </c>
-      <c r="N23" s="2">
+      <c r="P23" s="2">
         <v>1.0876187485279107</v>
       </c>
-      <c r="O23" s="2">
+      <c r="Q23" s="2">
         <v>1.0830712587251667</v>
       </c>
-      <c r="P23" s="2">
+      <c r="R23" s="2">
         <v>1.0799280197945567</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="S23" s="2">
         <v>1.0751292487075128</v>
       </c>
-      <c r="R23" s="2">
+      <c r="T23" s="2">
         <v>1.070534208732465</v>
       </c>
-      <c r="S23" s="2">
+      <c r="U23" s="2">
         <v>1.0660977065992343</v>
       </c>
-      <c r="T23" s="2">
+      <c r="V23" s="2">
         <v>1.0625365887255069</v>
       </c>
-      <c r="U23" s="2">
+      <c r="W23" s="2">
         <v>1.0618796840186346</v>
       </c>
-      <c r="V23" s="2">
+      <c r="X23" s="2">
         <v>1.05737460685317</v>
       </c>
-      <c r="W23" s="2">
+      <c r="Y23" s="2">
         <v>1.053558088927864</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -2313,47 +2468,53 @@
       <c r="J24" s="1">
         <v>3</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="1">
+        <v>4</v>
+      </c>
+      <c r="M24" s="2">
         <v>1.0157949365946117</v>
       </c>
-      <c r="L24" s="2">
+      <c r="N24" s="2">
         <v>1.0160462975141391</v>
       </c>
-      <c r="M24" s="2">
+      <c r="O24" s="2">
         <v>1.0127888140506438</v>
       </c>
-      <c r="N24" s="2">
+      <c r="P24" s="2">
         <v>1.013149162103866</v>
       </c>
-      <c r="O24" s="2">
+      <c r="Q24" s="2">
         <v>1.0127635511753779</v>
       </c>
-      <c r="P24" s="2">
+      <c r="R24" s="2">
         <v>1.0111531488925674</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="S24" s="2">
         <v>1.0115039821476666</v>
       </c>
-      <c r="R24" s="2">
+      <c r="T24" s="2">
         <v>1.0106295072115385</v>
       </c>
-      <c r="S24" s="2">
+      <c r="U24" s="2">
         <v>1.0098017621145376</v>
       </c>
-      <c r="T24" s="2">
+      <c r="V24" s="2">
         <v>1.0084003446295231</v>
       </c>
-      <c r="U24" s="2">
+      <c r="W24" s="2">
         <v>1.008188079842564</v>
       </c>
-      <c r="V24" s="2">
+      <c r="X24" s="2">
         <v>1.0091547356828192</v>
       </c>
-      <c r="W24" s="2">
+      <c r="Y24" s="2">
         <v>1.0084254516042059</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -2378,47 +2539,53 @@
       <c r="J25" s="1">
         <v>3</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="1">
+        <v>4</v>
+      </c>
+      <c r="M25" s="2">
         <v>1.0225641951351596</v>
       </c>
-      <c r="L25" s="2">
+      <c r="N25" s="2">
         <v>1.0211758516375116</v>
       </c>
-      <c r="M25" s="2">
+      <c r="O25" s="2">
         <v>1.0205899906215363</v>
       </c>
-      <c r="N25" s="2">
+      <c r="P25" s="2">
         <v>1.020034843205575</v>
       </c>
-      <c r="O25" s="2">
+      <c r="Q25" s="2">
         <v>1.0181759431294934</v>
       </c>
-      <c r="P25" s="2">
+      <c r="R25" s="2">
         <v>1.0184046661937418</v>
       </c>
-      <c r="Q25" s="2">
+      <c r="S25" s="2">
         <v>1.0172752106498404</v>
       </c>
-      <c r="R25" s="2">
+      <c r="T25" s="2">
         <v>1.0162635216346154</v>
       </c>
-      <c r="S25" s="2">
+      <c r="U25" s="2">
         <v>1.0158957415565344</v>
       </c>
-      <c r="T25" s="2">
+      <c r="V25" s="2">
         <v>1.0149698449167144</v>
       </c>
-      <c r="U25" s="2">
+      <c r="W25" s="2">
         <v>1.0146542029800394</v>
       </c>
-      <c r="V25" s="2">
+      <c r="X25" s="2">
         <v>1.0143171806167401</v>
       </c>
-      <c r="W25" s="2">
+      <c r="Y25" s="2">
         <v>1.0140536532758155</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -2443,47 +2610,53 @@
       <c r="J26" s="1">
         <v>3</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26" s="1">
+        <v>4</v>
+      </c>
+      <c r="M26" s="2">
         <v>1.0811061331685463</v>
       </c>
-      <c r="L26" s="2">
+      <c r="N26" s="2">
         <v>1.0762029174831265</v>
       </c>
-      <c r="M26" s="2">
+      <c r="O26" s="2">
         <v>1.0706131656299134</v>
       </c>
-      <c r="N26" s="2">
+      <c r="P26" s="2">
         <v>1.0668824862415023</v>
       </c>
-      <c r="O26" s="2">
+      <c r="Q26" s="2">
         <v>1.0604513867535823</v>
       </c>
-      <c r="P26" s="2">
+      <c r="R26" s="2">
         <v>1.0584963110434478</v>
       </c>
-      <c r="Q26" s="2">
+      <c r="S26" s="2">
         <v>1.0548824744570373</v>
       </c>
-      <c r="R26" s="2">
+      <c r="T26" s="2">
         <v>1.047151172104448</v>
       </c>
-      <c r="S26" s="2">
+      <c r="U26" s="2">
         <v>1.0468302658486708</v>
       </c>
-      <c r="T26" s="2">
+      <c r="V26" s="2">
         <v>1.0433693516699409</v>
       </c>
-      <c r="U26" s="2">
+      <c r="W26" s="2">
         <v>1.040975471430597</v>
       </c>
-      <c r="V26" s="2">
+      <c r="X26" s="2">
         <v>1.0394371328384717</v>
       </c>
-      <c r="W26" s="2">
+      <c r="Y26" s="2">
         <v>1.0358539478887472</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -2508,47 +2681,53 @@
       <c r="J27" s="1">
         <v>3</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="1">
+        <v>4</v>
+      </c>
+      <c r="M27" s="2">
         <v>0.95938444875671292</v>
       </c>
-      <c r="L27" s="2">
+      <c r="N27" s="2">
         <v>0.96128721118856575</v>
       </c>
-      <c r="M27" s="2">
+      <c r="O27" s="2">
         <v>0.96308295677380851</v>
       </c>
-      <c r="N27" s="2">
+      <c r="P27" s="2">
         <v>0.96474199435871899</v>
       </c>
-      <c r="O27" s="2">
+      <c r="Q27" s="2">
         <v>0.96566766297762352</v>
       </c>
-      <c r="P27" s="2">
+      <c r="R27" s="2">
         <v>0.96851107432805239</v>
       </c>
-      <c r="Q27" s="2">
+      <c r="S27" s="2">
         <v>0.96922011465507285</v>
       </c>
-      <c r="R27" s="2">
+      <c r="T27" s="2">
         <v>0.96995192307692313</v>
       </c>
-      <c r="S27" s="2">
+      <c r="U27" s="2">
         <v>0.97125550660792959</v>
       </c>
-      <c r="T27" s="2">
+      <c r="V27" s="2">
         <v>0.97250143595634686</v>
       </c>
-      <c r="U27" s="2">
+      <c r="W27" s="2">
         <v>0.97424093337081807</v>
       </c>
-      <c r="V27" s="2">
+      <c r="X27" s="2">
         <v>0.97535792951541844</v>
       </c>
-      <c r="W27" s="2">
+      <c r="Y27" s="2">
         <v>0.97644243731463998</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -2573,47 +2752,53 @@
       <c r="J28" s="1">
         <v>3</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="1">
+        <v>4</v>
+      </c>
+      <c r="M28" s="2">
         <v>1.0064753068522276</v>
       </c>
-      <c r="L28" s="2">
+      <c r="N28" s="2">
         <v>1.005957144127323</v>
       </c>
-      <c r="M28" s="2">
+      <c r="O28" s="2">
         <v>1.0054334403556433</v>
       </c>
-      <c r="N28" s="2">
+      <c r="P28" s="2">
         <v>1.0038375930616319</v>
       </c>
-      <c r="O28" s="2">
+      <c r="Q28" s="2">
         <v>1.0047495682210708</v>
       </c>
-      <c r="P28" s="2">
+      <c r="R28" s="2">
         <v>1.0056225443706814</v>
       </c>
-      <c r="Q28" s="2">
+      <c r="S28" s="2">
         <v>1.0053164232641558</v>
       </c>
-      <c r="R28" s="2">
+      <c r="T28" s="2">
         <v>1.0030343488287412</v>
       </c>
-      <c r="S28" s="2">
+      <c r="U28" s="2">
         <v>1.0028855032317636</v>
       </c>
-      <c r="T28" s="2">
+      <c r="V28" s="2">
         <v>1.0036859767838477</v>
       </c>
-      <c r="U28" s="2">
+      <c r="W28" s="2">
         <v>1.0035213118200452</v>
       </c>
-      <c r="V28" s="2">
+      <c r="X28" s="2">
         <v>1.00337361530715</v>
       </c>
-      <c r="W28" s="2">
+      <c r="Y28" s="2">
         <v>1.0032378098874015</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -2638,47 +2823,53 @@
       <c r="J29" s="1">
         <v>3</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="1">
+        <v>4</v>
+      </c>
+      <c r="M29" s="2">
         <v>0.97441220271672913</v>
       </c>
-      <c r="L29" s="2">
+      <c r="N29" s="2">
         <v>0.97663203121574815</v>
       </c>
-      <c r="M29" s="2">
+      <c r="O29" s="2">
         <v>0.97659647028732199</v>
       </c>
-      <c r="N29" s="2">
+      <c r="P29" s="2">
         <v>0.97859631657541057</v>
       </c>
-      <c r="O29" s="2">
+      <c r="Q29" s="2">
         <v>0.97911786089344865</v>
       </c>
-      <c r="P29" s="2">
+      <c r="R29" s="2">
         <v>0.98029478994246078</v>
       </c>
-      <c r="Q29" s="2">
+      <c r="S29" s="2">
         <v>0.98137816936631916</v>
       </c>
-      <c r="R29" s="2">
+      <c r="T29" s="2">
         <v>0.98121995192307687</v>
       </c>
-      <c r="S29" s="2">
+      <c r="U29" s="2">
         <v>0.98289280469897222</v>
       </c>
-      <c r="T29" s="2">
+      <c r="V29" s="2">
         <v>0.98266082711085578</v>
       </c>
-      <c r="U29" s="2">
+      <c r="W29" s="2">
         <v>0.98362384031487204</v>
       </c>
-      <c r="V29" s="2">
+      <c r="X29" s="2">
         <v>0.98451266519823788</v>
       </c>
-      <c r="W29" s="2">
+      <c r="Y29" s="2">
         <v>0.98540711782151524</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -2703,11 +2894,11 @@
       <c r="J30" s="1">
         <v>3</v>
       </c>
-      <c r="K30" s="2">
-        <v>1</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1</v>
+      <c r="K30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4</v>
       </c>
       <c r="M30" s="2">
         <v>1</v>
@@ -2742,8 +2933,14 @@
       <c r="W30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -2768,47 +2965,53 @@
       <c r="J31" s="1">
         <v>3</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" s="1">
+        <v>4</v>
+      </c>
+      <c r="M31" s="2">
         <v>0.97714211076280044</v>
       </c>
-      <c r="L31" s="2">
+      <c r="N31" s="2">
         <v>0.97833778163987339</v>
       </c>
-      <c r="M31" s="2">
+      <c r="O31" s="2">
         <v>0.98028885995027826</v>
       </c>
-      <c r="N31" s="2">
+      <c r="P31" s="2">
         <v>0.98206810725195159</v>
       </c>
-      <c r="O31" s="2">
+      <c r="Q31" s="2">
         <v>0.98289765654597616</v>
       </c>
-      <c r="P31" s="2">
+      <c r="R31" s="2">
         <v>0.98182762201453788</v>
       </c>
-      <c r="Q31" s="2">
+      <c r="S31" s="2">
         <v>0.98506940976730251</v>
       </c>
-      <c r="R31" s="2">
+      <c r="T31" s="2">
         <v>0.98475448468234505</v>
       </c>
-      <c r="S31" s="2">
+      <c r="U31" s="2">
         <v>0.98687323159701279</v>
       </c>
-      <c r="T31" s="2">
+      <c r="V31" s="2">
         <v>0.98803173607064421</v>
       </c>
-      <c r="U31" s="2">
+      <c r="W31" s="2">
         <v>0.9884638737097754</v>
       </c>
-      <c r="V31" s="2">
+      <c r="X31" s="2">
         <v>0.98949932795698925</v>
       </c>
-      <c r="W31" s="2">
+      <c r="Y31" s="2">
         <v>0.98982001791676844</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -2833,47 +3036,53 @@
       <c r="J32" s="1">
         <v>3</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="1">
+        <v>4</v>
+      </c>
+      <c r="M32" s="2">
         <v>0.94702498497467147</v>
       </c>
-      <c r="L32" s="2">
+      <c r="N32" s="2">
         <v>0.95340845520658513</v>
       </c>
-      <c r="M32" s="2">
+      <c r="O32" s="2">
         <v>0.95642424695418193</v>
       </c>
-      <c r="N32" s="2">
+      <c r="P32" s="2">
         <v>0.96022208166420697</v>
       </c>
-      <c r="O32" s="2">
+      <c r="Q32" s="2">
         <v>0.96352543272100266</v>
       </c>
-      <c r="P32" s="2">
+      <c r="R32" s="2">
         <v>0.96546961325966851</v>
       </c>
-      <c r="Q32" s="2">
+      <c r="S32" s="2">
         <v>0.96912511197372353</v>
       </c>
-      <c r="R32" s="2">
+      <c r="T32" s="2">
         <v>0.97155535328251219</v>
       </c>
-      <c r="S32" s="2">
+      <c r="U32" s="2">
         <v>0.9711017132942964</v>
       </c>
-      <c r="T32" s="2">
+      <c r="V32" s="2">
         <v>0.97237339967864</v>
       </c>
-      <c r="U32" s="2">
+      <c r="W32" s="2">
         <v>0.97351684388353366</v>
       </c>
-      <c r="V32" s="2">
+      <c r="X32" s="2">
         <v>0.97531394738098631</v>
       </c>
-      <c r="W32" s="2">
+      <c r="Y32" s="2">
         <v>0.97552351212343857</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2898,30 +3107,30 @@
       <c r="J33" s="1">
         <v>3</v>
       </c>
-      <c r="K33" s="2">
-        <v>1</v>
-      </c>
-      <c r="L33" s="2">
+      <c r="K33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" s="1">
+        <v>4</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1</v>
+      </c>
+      <c r="N33" s="2">
         <v>0.99900688970268747</v>
       </c>
-      <c r="M33" s="2">
-        <v>1</v>
-      </c>
-      <c r="N33" s="2">
-        <v>1</v>
-      </c>
       <c r="O33" s="2">
+        <v>1</v>
+      </c>
+      <c r="P33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="2">
         <v>0.9990799372192456</v>
       </c>
-      <c r="P33" s="2">
+      <c r="R33" s="2">
         <v>0.99911734164070598</v>
       </c>
-      <c r="Q33" s="2">
-        <v>1</v>
-      </c>
-      <c r="R33" s="2">
-        <v>1</v>
-      </c>
       <c r="S33" s="2">
         <v>1</v>
       </c>
@@ -2937,8 +3146,14 @@
       <c r="W33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -2963,47 +3178,53 @@
       <c r="J34" s="1">
         <v>3</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="1">
+        <v>4</v>
+      </c>
+      <c r="M34" s="2">
         <v>0.97369014847240409</v>
       </c>
-      <c r="L34" s="2">
+      <c r="N34" s="2">
         <v>0.9751413915559648</v>
       </c>
-      <c r="M34" s="2">
+      <c r="O34" s="2">
         <v>0.97659647028732199</v>
       </c>
-      <c r="N34" s="2">
+      <c r="P34" s="2">
         <v>0.97789115646258495</v>
       </c>
-      <c r="O34" s="2">
+      <c r="Q34" s="2">
         <v>0.97847160513773335</v>
       </c>
-      <c r="P34" s="2">
+      <c r="R34" s="2">
         <v>0.98029478994246078</v>
       </c>
-      <c r="Q34" s="2">
+      <c r="S34" s="2">
         <v>0.9807625716594206</v>
       </c>
-      <c r="R34" s="2">
+      <c r="T34" s="2">
         <v>0.98121995192307687</v>
       </c>
-      <c r="S34" s="2">
+      <c r="U34" s="2">
         <v>0.98226872246696051</v>
       </c>
-      <c r="T34" s="2">
+      <c r="V34" s="2">
         <v>0.9832711085582998</v>
       </c>
-      <c r="U34" s="2">
+      <c r="W34" s="2">
         <v>0.98418611189204386</v>
       </c>
-      <c r="V34" s="2">
+      <c r="X34" s="2">
         <v>0.98509774229074887</v>
       </c>
-      <c r="W34" s="2">
+      <c r="Y34" s="2">
         <v>0.98540711782151524</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
@@ -3028,47 +3249,53 @@
       <c r="J35" s="1">
         <v>3</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="1">
+        <v>4</v>
+      </c>
+      <c r="M35" s="2">
         <v>1.0013695319423186</v>
       </c>
-      <c r="L35" s="2">
-        <v>1</v>
-      </c>
-      <c r="M35" s="2">
-        <v>1</v>
-      </c>
       <c r="N35" s="2">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2">
+        <v>1</v>
+      </c>
+      <c r="P35" s="2">
         <v>1.0011362117363989</v>
       </c>
-      <c r="O35" s="2">
+      <c r="Q35" s="2">
         <v>0.99892486718947637</v>
       </c>
-      <c r="P35" s="2">
+      <c r="R35" s="2">
         <v>1.0010223719028144</v>
       </c>
-      <c r="Q35" s="2">
+      <c r="S35" s="2">
         <v>1.0009745471222196</v>
       </c>
-      <c r="R35" s="2">
+      <c r="T35" s="2">
         <v>1.0008761842177318</v>
       </c>
-      <c r="S35" s="2">
+      <c r="U35" s="2">
         <v>1.0008379595684507</v>
       </c>
-      <c r="T35" s="2">
+      <c r="V35" s="2">
         <v>1.000854571959986</v>
       </c>
-      <c r="U35" s="2">
+      <c r="W35" s="2">
         <v>1.0008215338520272</v>
       </c>
-      <c r="V35" s="2">
+      <c r="X35" s="2">
         <v>1.0007450176941703</v>
       </c>
-      <c r="W35" s="2">
+      <c r="Y35" s="2">
         <v>1.0007182618064285</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -3093,47 +3320,53 @@
       <c r="J36" s="1">
         <v>3</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L36" s="1">
+        <v>4</v>
+      </c>
+      <c r="M36" s="2">
         <v>0.96136344122950101</v>
       </c>
-      <c r="L36" s="2">
+      <c r="N36" s="2">
         <v>0.96539598817230077</v>
       </c>
-      <c r="M36" s="2">
+      <c r="O36" s="2">
         <v>0.96890649525375583</v>
       </c>
-      <c r="N36" s="2">
+      <c r="P36" s="2">
         <v>0.9718883969358354</v>
       </c>
-      <c r="O36" s="2">
+      <c r="Q36" s="2">
         <v>0.97453412029975461</v>
       </c>
-      <c r="P36" s="2">
+      <c r="R36" s="2">
         <v>0.97488699146157709</v>
       </c>
-      <c r="Q36" s="2">
+      <c r="S36" s="2">
         <v>0.97808300985368757</v>
       </c>
-      <c r="R36" s="2">
+      <c r="T36" s="2">
         <v>0.97815451132096942</v>
       </c>
-      <c r="S36" s="2">
+      <c r="U36" s="2">
         <v>0.97923443938408161</v>
       </c>
-      <c r="T36" s="2">
+      <c r="V36" s="2">
         <v>0.97931892396205877</v>
       </c>
-      <c r="U36" s="2">
+      <c r="W36" s="2">
         <v>0.98017489814170722</v>
       </c>
-      <c r="V36" s="2">
+      <c r="X36" s="2">
         <v>0.98090053955975731</v>
       </c>
-      <c r="W36" s="2">
+      <c r="Y36" s="2">
         <v>0.98085047759000743</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
@@ -3158,47 +3391,53 @@
       <c r="J37" s="1">
         <v>3</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="1">
+        <v>4</v>
+      </c>
+      <c r="M37" s="2">
         <v>0.99097432194593627</v>
       </c>
-      <c r="L37" s="2">
+      <c r="N37" s="2">
         <v>0.99193300889999558</v>
       </c>
-      <c r="M37" s="2">
+      <c r="O37" s="2">
         <v>0.99219882342910737</v>
       </c>
-      <c r="N37" s="2">
+      <c r="P37" s="2">
         <v>0.99170399867263981</v>
       </c>
-      <c r="O37" s="2">
+      <c r="Q37" s="2">
         <v>0.99192180305355848</v>
       </c>
-      <c r="P37" s="2">
+      <c r="R37" s="2">
         <v>0.99278789311894067</v>
       </c>
-      <c r="Q37" s="2">
+      <c r="S37" s="2">
         <v>0.99230502866376824</v>
       </c>
-      <c r="R37" s="2">
+      <c r="T37" s="2">
         <v>0.9930889423076924</v>
       </c>
-      <c r="S37" s="2">
+      <c r="U37" s="2">
         <v>0.99328193832599121</v>
       </c>
-      <c r="T37" s="2">
+      <c r="V37" s="2">
         <v>0.99343049971280861</v>
       </c>
-      <c r="U37" s="2">
+      <c r="W37" s="2">
         <v>0.99416643238684288</v>
       </c>
-      <c r="V37" s="2">
+      <c r="X37" s="2">
         <v>0.99370181718061679</v>
       </c>
-      <c r="W37" s="2">
+      <c r="Y37" s="2">
         <v>0.99440550013480722</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
@@ -3223,47 +3462,53 @@
       <c r="J38" s="1">
         <v>3</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L38" s="1">
+        <v>4</v>
+      </c>
+      <c r="M38" s="2">
         <v>1.0150277539600163</v>
       </c>
-      <c r="L38" s="2">
+      <c r="N38" s="2">
         <v>1.0145995001972905</v>
       </c>
-      <c r="M38" s="2">
+      <c r="O38" s="2">
         <v>1.0135135135135136</v>
       </c>
-      <c r="N38" s="2">
+      <c r="P38" s="2">
         <v>1.0138128422100547</v>
       </c>
-      <c r="O38" s="2">
+      <c r="Q38" s="2">
         <v>1.0114306486792148</v>
       </c>
-      <c r="P38" s="2">
+      <c r="R38" s="2">
         <v>1.0118231260345236</v>
       </c>
-      <c r="Q38" s="2">
+      <c r="S38" s="2">
         <v>1.0115039821476666</v>
       </c>
-      <c r="R38" s="2">
+      <c r="T38" s="2">
         <v>1.0099909855769231</v>
       </c>
-      <c r="S38" s="2">
+      <c r="U38" s="2">
         <v>1.0098017621145376</v>
       </c>
-      <c r="T38" s="2">
+      <c r="V38" s="2">
         <v>1.0089747271682941</v>
       </c>
-      <c r="U38" s="2">
+      <c r="W38" s="2">
         <v>1.0087854933933089</v>
       </c>
-      <c r="V38" s="2">
+      <c r="X38" s="2">
         <v>1.0086040748898679</v>
       </c>
-      <c r="W38" s="2">
+      <c r="Y38" s="2">
         <v>1.0084254516042059</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -3288,47 +3533,53 @@
       <c r="J39" s="1">
         <v>3</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L39" s="1">
+        <v>4</v>
+      </c>
+      <c r="M39" s="2">
         <v>0.98455121272980073</v>
       </c>
-      <c r="L39" s="2">
+      <c r="N39" s="2">
         <v>0.99034763045213736</v>
       </c>
-      <c r="M39" s="2">
+      <c r="O39" s="2">
         <v>0.99090846947843336</v>
       </c>
-      <c r="N39" s="2">
+      <c r="P39" s="2">
         <v>0.99138879896406595</v>
       </c>
-      <c r="O39" s="2">
+      <c r="Q39" s="2">
         <v>0.9928663673820799</v>
       </c>
-      <c r="P39" s="2">
+      <c r="R39" s="2">
         <v>0.99215364796814609</v>
       </c>
-      <c r="Q39" s="2">
+      <c r="S39" s="2">
         <v>0.99251856401094296</v>
       </c>
-      <c r="R39" s="2">
+      <c r="T39" s="2">
         <v>0.99199017461419348</v>
       </c>
-      <c r="S39" s="2">
+      <c r="U39" s="2">
         <v>0.99233128834355833</v>
       </c>
-      <c r="T39" s="2">
+      <c r="V39" s="2">
         <v>0.99179764243614943</v>
       </c>
-      <c r="U39" s="2">
+      <c r="W39" s="2">
         <v>0.99215463868802867</v>
       </c>
-      <c r="V39" s="2">
+      <c r="X39" s="2">
         <v>0.99239491780135713</v>
       </c>
-      <c r="W39" s="2">
+      <c r="Y39" s="2">
         <v>0.99121226767432669</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
@@ -3353,47 +3604,53 @@
       <c r="J40" s="1">
         <v>3</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L40" s="1">
+        <v>4</v>
+      </c>
+      <c r="M40" s="2">
         <v>1.020624131005716</v>
       </c>
-      <c r="L40" s="2">
+      <c r="N40" s="2">
         <v>1.0169097902605415</v>
       </c>
-      <c r="M40" s="2">
+      <c r="O40" s="2">
         <v>1.0159272677558275</v>
       </c>
-      <c r="N40" s="2">
+      <c r="P40" s="2">
         <v>1.0161864681126578</v>
       </c>
-      <c r="O40" s="2">
+      <c r="Q40" s="2">
         <v>1.016419654387799</v>
       </c>
-      <c r="P40" s="2">
+      <c r="R40" s="2">
         <v>1.0146387164773392</v>
       </c>
-      <c r="Q40" s="2">
+      <c r="S40" s="2">
         <v>1.0130087655630617</v>
       </c>
-      <c r="R40" s="2">
+      <c r="T40" s="2">
         <v>1.012441928765953</v>
       </c>
-      <c r="S40" s="2">
+      <c r="U40" s="2">
         <v>1.0110940695296524</v>
       </c>
-      <c r="T40" s="2">
+      <c r="V40" s="2">
         <v>1.0089882121807465</v>
       </c>
-      <c r="U40" s="2">
+      <c r="W40" s="2">
         <v>1.0070891819084078</v>
       </c>
-      <c r="V40" s="2">
+      <c r="X40" s="2">
         <v>1.0060567421102964</v>
       </c>
-      <c r="W40" s="2">
+      <c r="Y40" s="2">
         <v>1.0043938661628367</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -3418,47 +3675,53 @@
       <c r="J41" s="1">
         <v>3</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="1">
+        <v>4</v>
+      </c>
+      <c r="M41" s="2">
         <v>1.0924764890282133</v>
       </c>
-      <c r="L41" s="2">
+      <c r="N41" s="2">
         <v>1.0848488610266278</v>
       </c>
-      <c r="M41" s="2">
+      <c r="O41" s="2">
         <v>1.079910027228602</v>
       </c>
-      <c r="N41" s="2">
+      <c r="P41" s="2">
         <v>1.077271184523136</v>
       </c>
-      <c r="O41" s="2">
+      <c r="Q41" s="2">
         <v>1.0703577420576933</v>
       </c>
-      <c r="P41" s="2">
+      <c r="R41" s="2">
         <v>1.0657320872274143</v>
       </c>
-      <c r="Q41" s="2">
+      <c r="S41" s="2">
         <v>1.0624188554878657</v>
       </c>
-      <c r="R41" s="2">
+      <c r="T41" s="2">
         <v>1.0584812196412254</v>
       </c>
-      <c r="S41" s="2">
+      <c r="U41" s="2">
         <v>1.0548726749849251</v>
       </c>
-      <c r="T41" s="2">
+      <c r="V41" s="2">
         <v>1.0515038773589134</v>
       </c>
-      <c r="U41" s="2">
+      <c r="W41" s="2">
         <v>1.0491369589730246</v>
       </c>
-      <c r="V41" s="2">
+      <c r="X41" s="2">
         <v>1.0454889112903225</v>
       </c>
-      <c r="W41" s="2">
+      <c r="Y41" s="2">
         <v>1.0434074436028993</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -3483,47 +3746,53 @@
       <c r="J42" s="1">
         <v>3</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L42" s="1">
+        <v>4</v>
+      </c>
+      <c r="M42" s="2">
         <v>0.97517938535132465</v>
       </c>
-      <c r="L42" s="2">
+      <c r="N42" s="2">
         <v>0.97663203121574815</v>
       </c>
-      <c r="M42" s="2">
+      <c r="O42" s="2">
         <v>0.97800323983289295</v>
       </c>
-      <c r="N42" s="2">
+      <c r="P42" s="2">
         <v>0.97859631657541057</v>
       </c>
-      <c r="O42" s="2">
+      <c r="Q42" s="2">
         <v>0.97911786089344865</v>
       </c>
-      <c r="P42" s="2">
+      <c r="R42" s="2">
         <v>0.98029478994246078</v>
       </c>
-      <c r="Q42" s="2">
+      <c r="S42" s="2">
         <v>0.98137816936631916</v>
       </c>
-      <c r="R42" s="2">
+      <c r="T42" s="2">
         <v>0.98185847355769229</v>
       </c>
-      <c r="S42" s="2">
+      <c r="U42" s="2">
         <v>0.98289280469897222</v>
       </c>
-      <c r="T42" s="2">
+      <c r="V42" s="2">
         <v>0.98445577254451455</v>
       </c>
-      <c r="U42" s="2">
+      <c r="W42" s="2">
         <v>0.98478352544278891</v>
       </c>
-      <c r="V42" s="2">
+      <c r="X42" s="2">
         <v>0.98509774229074887</v>
       </c>
-      <c r="W42" s="2">
+      <c r="Y42" s="2">
         <v>0.98598004853060128</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -3554,47 +3823,53 @@
       <c r="J43" s="1">
         <v>3</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L43" s="1">
+        <v>4</v>
+      </c>
+      <c r="M43" s="2">
         <v>1.1381922675026124</v>
       </c>
-      <c r="L43" s="2">
+      <c r="N43" s="2">
         <v>1.126187077152256</v>
       </c>
-      <c r="M43" s="2">
+      <c r="O43" s="2">
         <v>1.1193323073280457</v>
       </c>
-      <c r="N43" s="2">
+      <c r="P43" s="2">
         <v>1.1121167552890598</v>
       </c>
-      <c r="O43" s="2">
+      <c r="Q43" s="2">
         <v>1.1054824917464956</v>
       </c>
-      <c r="P43" s="2">
+      <c r="R43" s="2">
         <v>1.0985981308411215</v>
       </c>
-      <c r="Q43" s="2">
+      <c r="S43" s="2">
         <v>1.0923799061220414</v>
       </c>
-      <c r="R43" s="2">
+      <c r="T43" s="2">
         <v>1.0865195017553984</v>
       </c>
-      <c r="S43" s="2">
+      <c r="U43" s="2">
         <v>1.0819147455818914</v>
       </c>
-      <c r="T43" s="2">
+      <c r="V43" s="2">
         <v>1.0761576045542156</v>
       </c>
-      <c r="U43" s="2">
+      <c r="W43" s="2">
         <v>1.0722525804493017</v>
       </c>
-      <c r="V43" s="2">
+      <c r="X43" s="2">
         <v>1.0685903897849462</v>
       </c>
-      <c r="W43" s="2">
+      <c r="Y43" s="2">
         <v>1.0590031761544101</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
@@ -3619,47 +3894,53 @@
       <c r="J44" s="1">
         <v>3</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L44" s="1">
+        <v>4</v>
+      </c>
+      <c r="M44" s="2">
         <v>0.99020713931134086</v>
       </c>
-      <c r="L44" s="2">
+      <c r="N44" s="2">
         <v>0.99193300889999558</v>
       </c>
-      <c r="M44" s="2">
+      <c r="O44" s="2">
         <v>0.99147412396623757</v>
       </c>
-      <c r="N44" s="2">
+      <c r="P44" s="2">
         <v>0.99170399867263981</v>
       </c>
-      <c r="O44" s="2">
+      <c r="Q44" s="2">
         <v>0.99192180305355848</v>
       </c>
-      <c r="P44" s="2">
+      <c r="R44" s="2">
         <v>0.99211791597698429</v>
       </c>
-      <c r="Q44" s="2">
+      <c r="S44" s="2">
         <v>0.99230502866376824</v>
       </c>
-      <c r="R44" s="2">
+      <c r="T44" s="2">
         <v>0.99184945913461542</v>
       </c>
-      <c r="S44" s="2">
+      <c r="U44" s="2">
         <v>0.99144640234948611</v>
       </c>
-      <c r="T44" s="2">
+      <c r="V44" s="2">
         <v>0.99224583572659386</v>
       </c>
-      <c r="U44" s="2">
+      <c r="W44" s="2">
         <v>0.99297160528535289</v>
       </c>
-      <c r="V44" s="2">
+      <c r="X44" s="2">
         <v>0.9931167400881058</v>
       </c>
-      <c r="W44" s="2">
+      <c r="Y44" s="2">
         <v>0.99325963871663525</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>70</v>
       </c>
@@ -3684,47 +3965,53 @@
       <c r="J45" s="1">
         <v>3</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L45" s="1">
+        <v>4</v>
+      </c>
+      <c r="M45" s="2">
         <v>1.1106878306878307</v>
       </c>
-      <c r="L45" s="2">
+      <c r="N45" s="2">
         <v>1.1043779371753648</v>
       </c>
-      <c r="M45" s="2">
+      <c r="O45" s="2">
         <v>1.0984562193455014</v>
       </c>
-      <c r="N45" s="2">
+      <c r="P45" s="2">
         <v>1.0968045850671273</v>
       </c>
-      <c r="O45" s="2">
+      <c r="Q45" s="2">
         <v>1.0913553731686736</v>
       </c>
-      <c r="P45" s="2">
+      <c r="R45" s="2">
         <v>1.0874259578615881</v>
       </c>
-      <c r="Q45" s="2">
+      <c r="S45" s="2">
         <v>1.083709162908371</v>
       </c>
-      <c r="R45" s="2">
+      <c r="T45" s="2">
         <v>1.079503462131812</v>
       </c>
-      <c r="S45" s="2">
+      <c r="U45" s="2">
         <v>1.0772310610051627</v>
       </c>
-      <c r="T45" s="2">
+      <c r="V45" s="2">
         <v>1.0734529425944419</v>
       </c>
-      <c r="U45" s="2">
+      <c r="W45" s="2">
         <v>1.0714333940989804</v>
       </c>
-      <c r="V45" s="2">
+      <c r="X45" s="2">
         <v>1.0678695580201956</v>
       </c>
-      <c r="W45" s="2">
+      <c r="Y45" s="2">
         <v>1.0659975965442203</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>67</v>
       </c>
@@ -3749,47 +4036,53 @@
       <c r="J46" s="1">
         <v>3</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="1">
+        <v>4</v>
+      </c>
+      <c r="M46" s="2">
         <v>1.1903735632183909</v>
       </c>
-      <c r="L46" s="2">
+      <c r="N46" s="2">
         <v>1.1778908820060827</v>
       </c>
-      <c r="M46" s="2">
+      <c r="O46" s="2">
         <v>1.1656801231206348</v>
       </c>
-      <c r="N46" s="2">
+      <c r="P46" s="2">
         <v>1.1554474488064259</v>
       </c>
-      <c r="O46" s="2">
+      <c r="Q46" s="2">
         <v>1.1451534339990257</v>
       </c>
-      <c r="P46" s="2">
+      <c r="R46" s="2">
         <v>1.1340602284527517</v>
       </c>
-      <c r="Q46" s="2">
+      <c r="S46" s="2">
         <v>1.1264855687606112</v>
       </c>
-      <c r="R46" s="2">
+      <c r="T46" s="2">
         <v>1.1169624392824509</v>
       </c>
-      <c r="S46" s="2">
+      <c r="U46" s="2">
         <v>1.1112760332111877</v>
       </c>
-      <c r="T46" s="2">
+      <c r="V46" s="2">
         <v>1.1045318033080818</v>
       </c>
-      <c r="U46" s="2">
+      <c r="W46" s="2">
         <v>1.0975800156128026</v>
       </c>
-      <c r="V46" s="2">
+      <c r="X46" s="2">
         <v>1.0909778225806452</v>
       </c>
-      <c r="W46" s="2">
+      <c r="Y46" s="2">
         <v>1.0861633683524716</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>76</v>
       </c>
@@ -3814,47 +4107,53 @@
       <c r="J47" s="1">
         <v>3</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L47" s="1">
+        <v>4</v>
+      </c>
+      <c r="M47" s="2">
         <v>0.70733304233958971</v>
       </c>
-      <c r="L47" s="2">
+      <c r="N47" s="2">
         <v>0.73722844955857558</v>
       </c>
-      <c r="M47" s="2">
+      <c r="O47" s="2">
         <v>0.76366281713194506</v>
       </c>
-      <c r="N47" s="2">
+      <c r="P47" s="2">
         <v>0.7857443052870472</v>
       </c>
-      <c r="O47" s="2">
+      <c r="Q47" s="2">
         <v>0.80571205007824731</v>
       </c>
-      <c r="P47" s="2">
+      <c r="R47" s="2">
         <v>0.82192783429700655</v>
       </c>
-      <c r="Q47" s="2">
+      <c r="S47" s="2">
         <v>0.83734359961501448</v>
       </c>
-      <c r="R47" s="2">
+      <c r="T47" s="2">
         <v>0.8486244484817026</v>
       </c>
-      <c r="S47" s="2">
+      <c r="U47" s="2">
         <v>0.85981078756604012</v>
       </c>
-      <c r="T47" s="2">
+      <c r="V47" s="2">
         <v>0.87080027998133469</v>
       </c>
-      <c r="U47" s="2">
+      <c r="W47" s="2">
         <v>0.87547754830850999</v>
       </c>
-      <c r="V47" s="2">
+      <c r="X47" s="2">
         <v>0.88138185654008427</v>
       </c>
-      <c r="W47" s="2">
+      <c r="Y47" s="2">
         <v>0.89259818731117824</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
@@ -3879,43 +4178,49 @@
       <c r="J48" s="1">
         <v>3</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="1">
+        <v>4</v>
+      </c>
+      <c r="M48" s="2">
         <v>1.2735210561497325</v>
       </c>
-      <c r="L48" s="2">
+      <c r="N48" s="2">
         <v>1.2600774403912778</v>
       </c>
-      <c r="M48" s="2">
+      <c r="O48" s="2">
         <v>1.2488874761602033</v>
       </c>
-      <c r="N48" s="2">
+      <c r="P48" s="2">
         <v>1.2387480097860277</v>
       </c>
-      <c r="O48" s="2">
+      <c r="Q48" s="2">
         <v>1.2301240939622784</v>
       </c>
-      <c r="P48" s="2">
+      <c r="R48" s="2">
         <v>1.2175800526882119</v>
       </c>
-      <c r="Q48" s="2">
+      <c r="S48" s="2">
         <v>1.209126854572496</v>
       </c>
-      <c r="R48" s="2">
+      <c r="T48" s="2">
         <v>1.2000355239786857</v>
       </c>
-      <c r="S48" s="2">
+      <c r="U48" s="2">
         <v>1.1905308165606423</v>
       </c>
-      <c r="T48" s="2">
+      <c r="V48" s="2">
         <v>1.1828998056796101</v>
       </c>
-      <c r="U48" s="2">
+      <c r="W48" s="2">
         <v>1.1759927797833933</v>
       </c>
-      <c r="V48" s="2">
+      <c r="X48" s="2">
         <v>1.1682678120594119</v>
       </c>
-      <c r="W48" s="2">
+      <c r="Y48" s="2">
         <v>1.1612592044760282</v>
       </c>
     </row>
@@ -3928,297 +4233,408 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F8FD4-18FD-46B0-89C5-E92BB2B9F58E}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="7">
         <v>85.1327</v>
       </c>
-      <c r="C2" s="7">
-        <v>40</v>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D2" s="7">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E2" s="7">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7">
         <v>26</v>
       </c>
-      <c r="F2" s="7">
+      <c r="G2" s="7">
         <v>1.6</v>
       </c>
-      <c r="G2" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="7">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="7">
         <v>110.1088</v>
       </c>
-      <c r="C3" s="7">
-        <v>40</v>
+      <c r="C3" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D3" s="7">
+        <v>40</v>
+      </c>
+      <c r="E3" s="7">
         <v>5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="7">
         <v>26</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>1.6</v>
       </c>
-      <c r="G3" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="7">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="7">
         <v>113.164</v>
       </c>
-      <c r="C4" s="7">
-        <v>40</v>
+      <c r="C4" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D4" s="7">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E4" s="7">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7">
         <v>26</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>1.6</v>
       </c>
-      <c r="G4" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="7">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="7">
         <v>117.0856</v>
       </c>
-      <c r="C5" s="7">
-        <v>40</v>
+      <c r="C5" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D5" s="7">
+        <v>40</v>
+      </c>
+      <c r="E5" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>26</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>1.6</v>
       </c>
-      <c r="G5" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="7">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="7">
         <v>135.09180000000001</v>
       </c>
-      <c r="C6" s="7">
-        <v>40</v>
+      <c r="C6" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D6" s="7">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E6" s="7">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7">
         <v>26</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>1.6</v>
       </c>
-      <c r="G6" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="7">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="7">
         <v>157.07429999999999</v>
       </c>
-      <c r="C7" s="7">
-        <v>40</v>
+      <c r="C7" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D7" s="7">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7">
         <v>5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>26</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>1.6</v>
       </c>
-      <c r="G7" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="7">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="7">
         <v>165.1318</v>
       </c>
-      <c r="C8" s="7">
-        <v>40</v>
+      <c r="C8" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D8" s="7">
+        <v>40</v>
+      </c>
+      <c r="E8" s="7">
         <v>5</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>30</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>1.6</v>
       </c>
-      <c r="G8" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="7">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="7">
         <v>173.11179999999999</v>
       </c>
-      <c r="C9" s="7">
-        <v>40</v>
+      <c r="C9" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D9" s="7">
+        <v>40</v>
+      </c>
+      <c r="E9" s="7">
         <v>5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>30</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="7">
         <v>1.6</v>
       </c>
-      <c r="G9" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="7">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="7">
         <v>184.07740000000001</v>
       </c>
-      <c r="C10" s="7">
-        <v>40</v>
+      <c r="C10" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="7">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7">
         <v>10</v>
       </c>
-      <c r="E10" s="7">
-        <v>40</v>
-      </c>
       <c r="F10" s="7">
+        <v>40</v>
+      </c>
+      <c r="G10" s="7">
         <v>1.6</v>
       </c>
-      <c r="G10" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="7">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B11" s="7">
         <v>200.07230000000001</v>
       </c>
-      <c r="C11" s="7">
-        <v>40</v>
+      <c r="C11" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D11" s="7">
+        <v>40</v>
+      </c>
+      <c r="E11" s="7">
         <v>10</v>
       </c>
-      <c r="E11" s="7">
-        <v>40</v>
-      </c>
       <c r="F11" s="7">
+        <v>40</v>
+      </c>
+      <c r="G11" s="7">
         <v>1.6</v>
       </c>
-      <c r="G11" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="7">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="7">
         <v>216.0427</v>
       </c>
-      <c r="C12" s="7">
-        <v>40</v>
+      <c r="C12" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D12" s="7">
+        <v>40</v>
+      </c>
+      <c r="E12" s="7">
         <v>10</v>
       </c>
-      <c r="E12" s="7">
-        <v>40</v>
-      </c>
       <c r="F12" s="7">
+        <v>40</v>
+      </c>
+      <c r="G12" s="7">
         <v>1.6</v>
       </c>
-      <c r="G12" s="7">
-        <v>20</v>
+      <c r="H12" s="7">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4228,10 +4644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFFE8E4-84E1-4284-A5B8-07DB42525DFD}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,14 +4655,13 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -4268,11 +4683,8 @@
       <c r="G1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>13</v>
       </c>
@@ -4283,18 +4695,15 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>4</v>
+        <v>121.0509</v>
       </c>
       <c r="E2" s="1">
-        <v>121.0509</v>
+        <v>922.00980000000004</v>
       </c>
       <c r="F2" s="1">
-        <v>922.00980000000004</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1">
-        <v>100</v>
-      </c>
-      <c r="H2" s="1">
         <v>1000</v>
       </c>
     </row>

</xml_diff>